<commit_message>
Tablero listo para despliegue en UPN
</commit_message>
<xml_diff>
--- a/informes/Encuesta de satisfacción del servicio de transporte.xlsx
+++ b/informes/Encuesta de satisfacción del servicio de transporte.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27823"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27909"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qinzen\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BABE7047-C8DF-4791-98A5-98AD245F3E9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D72776D5-740B-4B55-AAD9-94BA43956512}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13905" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="202">
   <si>
     <t>ID</t>
   </si>
@@ -626,6 +626,21 @@
   </si>
   <si>
     <t>Huele a gasolina.</t>
+  </si>
+  <si>
+    <t>GRUPO DE ASEGURAMIENTO DE LA CALIDAD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Angie Manrique </t>
+  </si>
+  <si>
+    <t>Administrativo Provisional</t>
+  </si>
+  <si>
+    <t>OFICINA DE CONTROL INTERNO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Claudia Rojas </t>
   </si>
   <si>
     <t>nGREgiPT_k6Tg1M4a_CM6ISJUD-DI7NBoIgAQxXYz_hUMTdPVkhHNklaVjdQQjcyVFZFS0kwNlFTMSQlQCN0PWcu</t>
@@ -791,8 +806,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:AE29" totalsRowShown="0">
-  <autoFilter ref="A1:AE29" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:AE31" totalsRowShown="0">
+  <autoFilter ref="A1:AE31" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="31">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="30"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Hora de inicio" dataDxfId="29"/>
@@ -1127,7 +1142,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AE29"/>
+  <dimension ref="A1:AE31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="I1" sqref="I1"/>
@@ -3591,6 +3606,177 @@
       </c>
       <c r="AD29" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:31">
+      <c r="A30">
+        <v>31</v>
+      </c>
+      <c r="B30" s="1">
+        <v>45476.600208333337</v>
+      </c>
+      <c r="C30" s="1">
+        <v>45476.612546296295</v>
+      </c>
+      <c r="D30" t="s">
+        <v>185</v>
+      </c>
+      <c r="F30" s="1"/>
+      <c r="G30" t="s">
+        <v>33</v>
+      </c>
+      <c r="H30" t="s">
+        <v>87</v>
+      </c>
+      <c r="I30" t="s">
+        <v>35</v>
+      </c>
+      <c r="J30" t="s">
+        <v>36</v>
+      </c>
+      <c r="K30" t="s">
+        <v>56</v>
+      </c>
+      <c r="L30" t="s">
+        <v>38</v>
+      </c>
+      <c r="M30" t="s">
+        <v>39</v>
+      </c>
+      <c r="N30" t="s">
+        <v>194</v>
+      </c>
+      <c r="O30" t="s">
+        <v>195</v>
+      </c>
+      <c r="P30" s="2">
+        <v>45476</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>42</v>
+      </c>
+      <c r="R30" t="s">
+        <v>96</v>
+      </c>
+      <c r="S30" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="T30" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="U30" t="s">
+        <v>116</v>
+      </c>
+      <c r="V30" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="W30" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="X30" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y30" t="s">
+        <v>116</v>
+      </c>
+      <c r="Z30" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA30" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB30" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC30" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD30" t="s">
+        <v>33</v>
+      </c>
+      <c r="AE30" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="31" spans="1:31">
+      <c r="A31">
+        <v>32</v>
+      </c>
+      <c r="B31" s="1">
+        <v>45482.464513888888</v>
+      </c>
+      <c r="C31" s="1">
+        <v>45482.466122685182</v>
+      </c>
+      <c r="D31" t="s">
+        <v>185</v>
+      </c>
+      <c r="F31" s="1"/>
+      <c r="G31" t="s">
+        <v>33</v>
+      </c>
+      <c r="H31" t="s">
+        <v>196</v>
+      </c>
+      <c r="I31" t="s">
+        <v>133</v>
+      </c>
+      <c r="J31" t="s">
+        <v>36</v>
+      </c>
+      <c r="K31" t="s">
+        <v>37</v>
+      </c>
+      <c r="L31" t="s">
+        <v>38</v>
+      </c>
+      <c r="M31" t="s">
+        <v>39</v>
+      </c>
+      <c r="N31" t="s">
+        <v>197</v>
+      </c>
+      <c r="O31" t="s">
+        <v>198</v>
+      </c>
+      <c r="P31" s="2">
+        <v>45469</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>42</v>
+      </c>
+      <c r="R31" t="s">
+        <v>192</v>
+      </c>
+      <c r="S31" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="T31" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="V31" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="W31" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="X31" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z31" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA31" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB31" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC31" t="s">
+        <v>48</v>
+      </c>
+      <c r="AD31" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -3612,17 +3798,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -3632,6 +3818,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101003D45681223310045808A22EA47D7845F" ma:contentTypeVersion="4" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="9b9450793f3d36e97df90e069ade6c5b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0c2a4331-f396-4bb5-9ba8-7f95892487d8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8d9c68a369494e1f3cefcf3e5a9d305c" ns2:_="">
     <xsd:import namespace="0c2a4331-f396-4bb5-9ba8-7f95892487d8"/>
@@ -3775,29 +3970,20 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3319C442-CA14-4432-988E-65269E15CEAF}"/>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F9B834CB-30B8-47F7-828A-C420AC525921}"/>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97F94192-ACE3-4F6C-BC44-CE65402515D2}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3319C442-CA14-4432-988E-65269E15CEAF}"/>
 </file>
</xml_diff>